<commit_message>
Students can now change profile picture
</commit_message>
<xml_diff>
--- a/src/main/resources/UMS_Data.xlsx
+++ b/src/main/resources/UMS_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\IdeaProjects\UniversityManagementApplication\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\IdeaProjects\UniversityManagementAppl\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C811FA49-31F4-41E1-B0B0-5DAE78129E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2566783C-922F-4780-AB04-4D9D28EE9B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3390" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Subjects" sheetId="1" r:id="rId1"/>
@@ -4952,7 +4952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -8889,8 +8889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Faculty and student profile picture paths get exported
</commit_message>
<xml_diff>
--- a/src/main/resources/UMS_Data.xlsx
+++ b/src/main/resources/UMS_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\IdeaProjects\UniversityManagementAppl\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2566783C-922F-4780-AB04-4D9D28EE9B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BA0B99-14C8-4C4F-9613-A0A38D18D52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Subjects" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="184">
   <si>
     <t>Subject Code</t>
   </si>
@@ -578,6 +578,9 @@
   </si>
   <si>
     <t>Alice Smith, Bob Johnson, Lucka Racki,Helen Jones,David Lee</t>
+  </si>
+  <si>
+    <t>Profile Picture</t>
   </si>
 </sst>
 </file>
@@ -653,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -676,6 +679,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4952,7 +4956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -7724,10 +7728,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H1000"/>
+  <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -7743,7 +7747,7 @@
     <col min="9" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>138</v>
       </c>
@@ -7768,8 +7772,11 @@
       <c r="H1" s="7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="I1" s="14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>143</v>
       </c>
@@ -7795,7 +7802,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>147</v>
       </c>
@@ -7821,7 +7828,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>151</v>
       </c>
@@ -7847,7 +7854,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>157</v>
       </c>
@@ -7873,7 +7880,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>159</v>
       </c>
@@ -8889,7 +8896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated exporter for registered courses
</commit_message>
<xml_diff>
--- a/src/main/resources/UMS_Data.xlsx
+++ b/src/main/resources/UMS_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\IdeaProjects\UniversityManagementAppl\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BA0B99-14C8-4C4F-9613-A0A38D18D52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D861BC43-07F3-4954-852F-91746CD5CC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Subjects" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="183">
   <si>
     <t>Subject Code</t>
   </si>
@@ -578,9 +578,6 @@
   </si>
   <si>
     <t>Alice Smith, Bob Johnson, Lucka Racki,Helen Jones,David Lee</t>
-  </si>
-  <si>
-    <t>Profile Picture</t>
   </si>
 </sst>
 </file>
@@ -656,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -679,7 +676,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6290,8 +6286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -7728,10 +7724,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -7747,8 +7743,8 @@
     <col min="9" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -7772,11 +7768,8 @@
       <c r="H1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>143</v>
       </c>
@@ -7795,14 +7788,14 @@
       <c r="F2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>147</v>
       </c>
@@ -7821,14 +7814,14 @@
       <c r="F3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>151</v>
       </c>
@@ -7847,14 +7840,14 @@
       <c r="F4" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="4" t="s">
         <v>156</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>157</v>
       </c>
@@ -7880,7 +7873,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>159</v>
       </c>
@@ -8896,9 +8889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>